<commit_message>
Added 1206 resistor networks to minimize component count on board
</commit_message>
<xml_diff>
--- a/calculation.xlsx
+++ b/calculation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\eagle\projects\Pi_Interface\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C774CB6-E7B9-4D1A-85CE-1A81FDBB7F04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED97AD28-18CD-4DE4-9798-36435883FE53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{923AA141-4759-4248-8827-CC87707017B5}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Part</t>
   </si>
@@ -112,6 +112,12 @@
   </si>
   <si>
     <t>Zener diode 5.1V</t>
+  </si>
+  <si>
+    <t>BZT52C3V6</t>
+  </si>
+  <si>
+    <t>C173412</t>
   </si>
 </sst>
 </file>
@@ -484,7 +490,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -710,11 +716,17 @@
         <v>25</v>
       </c>
       <c r="C13" s="1">
-        <v>0.08</v>
+        <v>1.5599999999999999E-2</v>
       </c>
       <c r="D13" s="1">
         <f t="shared" si="0"/>
-        <v>0.16</v>
+        <v>3.1199999999999999E-2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -761,7 +773,7 @@
     <row r="21" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D21" s="2">
         <f>SUM(D2:D19)</f>
-        <v>6.6406000000000009</v>
+        <v>6.5118000000000009</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed Layout, added EEPROM
</commit_message>
<xml_diff>
--- a/calculation.xlsx
+++ b/calculation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\eagle\projects\Pi_Interface\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED97AD28-18CD-4DE4-9798-36435883FE53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34FD25A0-AFE7-4F29-9EB2-9CFFFC2DB05D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{923AA141-4759-4248-8827-CC87707017B5}"/>
+    <workbookView xWindow="-25320" yWindow="195" windowWidth="25440" windowHeight="15390" xr2:uid="{923AA141-4759-4248-8827-CC87707017B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Part</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>C173412</t>
+  </si>
+  <si>
+    <t>LTV-247</t>
   </si>
 </sst>
 </file>
@@ -490,7 +493,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,6 +554,9 @@
         <f t="shared" ref="D3:D19" si="0">C3*A3</f>
         <v>0.57399999999999995</v>
       </c>
+      <c r="E3" t="s">
+        <v>28</v>
+      </c>
       <c r="F3" t="s">
         <v>19</v>
       </c>

</xml_diff>